<commit_message>
ng: update ento forms
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2024/delta/nov 2024/ng_oncho_2411_1_community_del.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2024/delta/nov 2024/ng_oncho_2411_1_community_del.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2024\delta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2024\delta\nov 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CB8BD8-A89B-4A25-8EAF-C465F1050609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72D98D2-42FD-476D-A0DC-E26ED2A19A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">choices!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="265">
   <si>
     <t>type</t>
   </si>
@@ -461,9 +464,6 @@
     <t>ASHAKA</t>
   </si>
   <si>
-    <t>UTAGBAUNO</t>
-  </si>
-  <si>
     <t>ETUA</t>
   </si>
   <si>
@@ -509,9 +509,6 @@
     <t>OGBOLI</t>
   </si>
   <si>
-    <t>ILLA</t>
-  </si>
-  <si>
     <t>BOLU ANGIAMA</t>
   </si>
   <si>
@@ -584,9 +581,6 @@
     <t>DEL_ANN_N_013</t>
   </si>
   <si>
-    <t>DEL_ANN_N_014</t>
-  </si>
-  <si>
     <t>DEL_ANN_S_015</t>
   </si>
   <si>
@@ -827,10 +821,19 @@
     <t>DEL_WAN_M_094</t>
   </si>
   <si>
-    <t>(Delta) 1. Community Registration Form V2</t>
-  </si>
-  <si>
-    <t>ng_oncho_2408_1_community_del_v2</t>
+    <t>(Delta) 1. Community Registration Form V3</t>
+  </si>
+  <si>
+    <t>ng_oncho_2408_1_community_del_v3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTAGBAUNO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILLA </t>
+  </si>
+  <si>
+    <t>DEL_OSN_N_014</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1068,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
@@ -1410,7 +1434,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C25" sqref="C25:C26"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1759,11 +1783,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F203"/>
+  <dimension ref="A1:F202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F110" sqref="F110:F203"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A106" sqref="A106:XFD106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1796,7 +1820,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>43</v>
@@ -1810,31 +1834,34 @@
         <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1843,10 +1870,10 @@
         <v>57</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>68</v>
@@ -1857,10 +1884,10 @@
         <v>57</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>68</v>
@@ -1871,10 +1898,10 @@
         <v>57</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>68</v>
@@ -1884,13 +1911,13 @@
       <c r="A11" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1899,10 +1926,10 @@
         <v>57</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
         <v>68</v>
@@ -1913,10 +1940,10 @@
         <v>57</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
         <v>68</v>
@@ -1927,10 +1954,10 @@
         <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D14" t="s">
         <v>68</v>
@@ -1941,10 +1968,10 @@
         <v>57</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
         <v>68</v>
@@ -1955,10 +1982,10 @@
         <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D16" t="s">
         <v>68</v>
@@ -1969,10 +1996,10 @@
         <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D17" t="s">
         <v>68</v>
@@ -1983,10 +2010,10 @@
         <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D18" t="s">
         <v>68</v>
@@ -1997,10 +2024,10 @@
         <v>57</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D19" t="s">
         <v>68</v>
@@ -2011,10 +2038,10 @@
         <v>57</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D20" t="s">
         <v>68</v>
@@ -2025,10 +2052,10 @@
         <v>57</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
         <v>68</v>
@@ -2039,10 +2066,10 @@
         <v>57</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s">
         <v>68</v>
@@ -2053,10 +2080,10 @@
         <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D23" t="s">
         <v>68</v>
@@ -2067,10 +2094,10 @@
         <v>57</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D24" t="s">
         <v>68</v>
@@ -2081,27 +2108,27 @@
         <v>57</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D25" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D26" t="s">
-        <v>68</v>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2109,10 +2136,10 @@
         <v>62</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E28" t="s">
         <v>69</v>
@@ -2122,13 +2149,14 @@
       <c r="A29" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="B29" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2137,10 +2165,10 @@
         <v>62</v>
       </c>
       <c r="B30" s="25" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D30" s="26"/>
       <c r="E30" s="26" t="s">
@@ -2152,10 +2180,10 @@
         <v>62</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="26" t="s">
@@ -2167,10 +2195,10 @@
         <v>62</v>
       </c>
       <c r="B32" s="25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="26" t="s">
@@ -2182,10 +2210,10 @@
         <v>62</v>
       </c>
       <c r="B33" s="25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="26" t="s">
@@ -2197,10 +2225,10 @@
         <v>62</v>
       </c>
       <c r="B34" s="25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="26" t="s">
@@ -2212,10 +2240,10 @@
         <v>62</v>
       </c>
       <c r="B35" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="26" t="s">
@@ -2227,10 +2255,10 @@
         <v>62</v>
       </c>
       <c r="B36" s="25" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="D36" s="26"/>
       <c r="E36" s="26" t="s">
@@ -2242,10 +2270,10 @@
         <v>62</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D37" s="26"/>
       <c r="E37" s="26" t="s">
@@ -2257,10 +2285,10 @@
         <v>62</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D38" s="26"/>
       <c r="E38" s="26" t="s">
@@ -2272,10 +2300,10 @@
         <v>62</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D39" s="26"/>
       <c r="E39" s="26" t="s">
@@ -2287,14 +2315,14 @@
         <v>62</v>
       </c>
       <c r="B40" s="25" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="D40" s="26"/>
       <c r="E40" s="26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2302,14 +2330,14 @@
         <v>62</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="D41" s="26"/>
       <c r="E41" s="26" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2317,10 +2345,10 @@
         <v>62</v>
       </c>
       <c r="B42" s="25" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D42" s="26"/>
       <c r="E42" s="26" t="s">
@@ -2332,10 +2360,10 @@
         <v>62</v>
       </c>
       <c r="B43" s="25" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D43" s="26"/>
       <c r="E43" s="26" t="s">
@@ -2347,10 +2375,10 @@
         <v>62</v>
       </c>
       <c r="B44" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D44" s="26"/>
       <c r="E44" s="26" t="s">
@@ -2362,10 +2390,10 @@
         <v>62</v>
       </c>
       <c r="B45" s="25" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D45" s="26"/>
       <c r="E45" s="26" t="s">
@@ -2377,10 +2405,10 @@
         <v>62</v>
       </c>
       <c r="B46" s="25" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C46" s="25" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D46" s="26"/>
       <c r="E46" s="26" t="s">
@@ -2392,10 +2420,10 @@
         <v>62</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C47" s="25" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D47" s="26"/>
       <c r="E47" s="26" t="s">
@@ -2407,10 +2435,10 @@
         <v>62</v>
       </c>
       <c r="B48" s="25" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C48" s="25" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D48" s="26"/>
       <c r="E48" s="26" t="s">
@@ -2422,10 +2450,10 @@
         <v>62</v>
       </c>
       <c r="B49" s="25" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D49" s="26"/>
       <c r="E49" s="26" t="s">
@@ -2437,14 +2465,14 @@
         <v>62</v>
       </c>
       <c r="B50" s="25" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D50" s="26"/>
       <c r="E50" s="26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2452,14 +2480,14 @@
         <v>62</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D51" s="26"/>
       <c r="E51" s="26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2467,14 +2495,14 @@
         <v>62</v>
       </c>
       <c r="B52" s="25" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C52" s="25" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D52" s="26"/>
       <c r="E52" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -2482,14 +2510,14 @@
         <v>62</v>
       </c>
       <c r="B53" s="25" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C53" s="25" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D53" s="26"/>
       <c r="E53" s="26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -2497,10 +2525,10 @@
         <v>62</v>
       </c>
       <c r="B54" s="25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D54" s="26"/>
       <c r="E54" s="26" t="s">
@@ -2512,10 +2540,10 @@
         <v>62</v>
       </c>
       <c r="B55" s="25" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C55" s="25" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D55" s="26"/>
       <c r="E55" s="26" t="s">
@@ -2527,14 +2555,14 @@
         <v>62</v>
       </c>
       <c r="B56" s="25" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C56" s="25" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D56" s="26"/>
       <c r="E56" s="26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2542,14 +2570,14 @@
         <v>62</v>
       </c>
       <c r="B57" s="25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C57" s="25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D57" s="26"/>
       <c r="E57" s="26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2557,10 +2585,10 @@
         <v>62</v>
       </c>
       <c r="B58" s="25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C58" s="25" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D58" s="26"/>
       <c r="E58" s="26" t="s">
@@ -2572,10 +2600,10 @@
         <v>62</v>
       </c>
       <c r="B59" s="25" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C59" s="25" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D59" s="26"/>
       <c r="E59" s="26" t="s">
@@ -2587,10 +2615,10 @@
         <v>62</v>
       </c>
       <c r="B60" s="25" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C60" s="25" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D60" s="26"/>
       <c r="E60" s="26" t="s">
@@ -2602,10 +2630,10 @@
         <v>62</v>
       </c>
       <c r="B61" s="25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C61" s="25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D61" s="26"/>
       <c r="E61" s="26" t="s">
@@ -2617,14 +2645,14 @@
         <v>62</v>
       </c>
       <c r="B62" s="25" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="C62" s="25" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D62" s="26"/>
       <c r="E62" s="26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2632,14 +2660,14 @@
         <v>62</v>
       </c>
       <c r="B63" s="25" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C63" s="25" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="D63" s="26"/>
       <c r="E63" s="26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2647,10 +2675,10 @@
         <v>62</v>
       </c>
       <c r="B64" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C64" s="25" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D64" s="26"/>
       <c r="E64" s="26" t="s">
@@ -2662,10 +2690,10 @@
         <v>62</v>
       </c>
       <c r="B65" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C65" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D65" s="26"/>
       <c r="E65" s="26" t="s">
@@ -2677,14 +2705,14 @@
         <v>62</v>
       </c>
       <c r="B66" s="25" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C66" s="25" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D66" s="26"/>
       <c r="E66" s="26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2692,14 +2720,14 @@
         <v>62</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C67" s="25" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D67" s="26"/>
       <c r="E67" s="26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2707,14 +2735,14 @@
         <v>62</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D68" s="26"/>
       <c r="E68" s="26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2722,14 +2750,14 @@
         <v>62</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D69" s="26"/>
       <c r="E69" s="26" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2737,10 +2765,10 @@
         <v>62</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C70" s="25" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D70" s="26"/>
       <c r="E70" s="26" t="s">
@@ -2752,10 +2780,10 @@
         <v>62</v>
       </c>
       <c r="B71" s="25" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C71" s="25" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D71" s="26"/>
       <c r="E71" s="26" t="s">
@@ -2767,14 +2795,14 @@
         <v>62</v>
       </c>
       <c r="B72" s="25" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C72" s="25" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D72" s="26"/>
       <c r="E72" s="26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2782,14 +2810,14 @@
         <v>62</v>
       </c>
       <c r="B73" s="25" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C73" s="25" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D73" s="26"/>
       <c r="E73" s="26" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2797,14 +2825,14 @@
         <v>62</v>
       </c>
       <c r="B74" s="25" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C74" s="25" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D74" s="26"/>
       <c r="E74" s="26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2812,10 +2840,10 @@
         <v>62</v>
       </c>
       <c r="B75" s="25" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C75" s="25" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D75" s="26"/>
       <c r="E75" s="26" t="s">
@@ -2827,10 +2855,10 @@
         <v>62</v>
       </c>
       <c r="B76" s="25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C76" s="25" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D76" s="26"/>
       <c r="E76" s="26" t="s">
@@ -2842,10 +2870,10 @@
         <v>62</v>
       </c>
       <c r="B77" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C77" s="25" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D77" s="26"/>
       <c r="E77" s="26" t="s">
@@ -2857,10 +2885,10 @@
         <v>62</v>
       </c>
       <c r="B78" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C78" s="25" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D78" s="26"/>
       <c r="E78" s="26" t="s">
@@ -2872,14 +2900,14 @@
         <v>62</v>
       </c>
       <c r="B79" s="25" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C79" s="25" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D79" s="26"/>
       <c r="E79" s="26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2887,14 +2915,14 @@
         <v>62</v>
       </c>
       <c r="B80" s="25" t="s">
-        <v>136</v>
+        <v>262</v>
       </c>
       <c r="C80" s="25" t="s">
-        <v>136</v>
+        <v>262</v>
       </c>
       <c r="D80" s="26"/>
       <c r="E80" s="26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2909,7 +2937,7 @@
       </c>
       <c r="D81" s="26"/>
       <c r="E81" s="26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2917,14 +2945,14 @@
         <v>62</v>
       </c>
       <c r="B82" s="25" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="C82" s="25" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="D82" s="26"/>
       <c r="E82" s="26" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2932,14 +2960,14 @@
         <v>62</v>
       </c>
       <c r="B83" s="25" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C83" s="25" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D83" s="26"/>
       <c r="E83" s="26" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2947,10 +2975,10 @@
         <v>62</v>
       </c>
       <c r="B84" s="25" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C84" s="25" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D84" s="26"/>
       <c r="E84" s="26" t="s">
@@ -2962,10 +2990,10 @@
         <v>62</v>
       </c>
       <c r="B85" s="25" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C85" s="25" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D85" s="26"/>
       <c r="E85" s="26" t="s">
@@ -2977,10 +3005,10 @@
         <v>62</v>
       </c>
       <c r="B86" s="25" t="s">
-        <v>147</v>
+        <v>263</v>
       </c>
       <c r="C86" s="25" t="s">
-        <v>147</v>
+        <v>263</v>
       </c>
       <c r="D86" s="26"/>
       <c r="E86" s="26" t="s">
@@ -2992,10 +3020,10 @@
         <v>62</v>
       </c>
       <c r="B87" s="25" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C87" s="25" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D87" s="26"/>
       <c r="E87" s="26" t="s">
@@ -3007,10 +3035,10 @@
         <v>62</v>
       </c>
       <c r="B88" s="25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C88" s="25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D88" s="26"/>
       <c r="E88" s="26" t="s">
@@ -3037,10 +3065,10 @@
         <v>62</v>
       </c>
       <c r="B90" s="25" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="C90" s="25" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D90" s="26"/>
       <c r="E90" s="26" t="s">
@@ -3052,10 +3080,10 @@
         <v>62</v>
       </c>
       <c r="B91" s="25" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C91" s="25" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D91" s="26"/>
       <c r="E91" s="26" t="s">
@@ -3067,14 +3095,14 @@
         <v>62</v>
       </c>
       <c r="B92" s="25" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C92" s="25" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D92" s="26"/>
       <c r="E92" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3097,10 +3125,10 @@
         <v>62</v>
       </c>
       <c r="B94" s="25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C94" s="25" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D94" s="26"/>
       <c r="E94" s="26" t="s">
@@ -3127,10 +3155,10 @@
         <v>62</v>
       </c>
       <c r="B96" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C96" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D96" s="26"/>
       <c r="E96" s="26" t="s">
@@ -3142,14 +3170,14 @@
         <v>62</v>
       </c>
       <c r="B97" s="25" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C97" s="25" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D97" s="26"/>
       <c r="E97" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -3157,14 +3185,14 @@
         <v>62</v>
       </c>
       <c r="B98" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C98" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D98" s="26"/>
       <c r="E98" s="26" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -3172,10 +3200,10 @@
         <v>62</v>
       </c>
       <c r="B99" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C99" s="25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D99" s="26"/>
       <c r="E99" s="26" t="s">
@@ -3187,14 +3215,14 @@
         <v>62</v>
       </c>
       <c r="B100" s="25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C100" s="25" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D100" s="26"/>
       <c r="E100" s="26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -3202,10 +3230,10 @@
         <v>62</v>
       </c>
       <c r="B101" s="25" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C101" s="25" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D101" s="26"/>
       <c r="E101" s="26" t="s">
@@ -3217,10 +3245,10 @@
         <v>62</v>
       </c>
       <c r="B102" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C102" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D102" s="26"/>
       <c r="E102" s="26" t="s">
@@ -3232,14 +3260,14 @@
         <v>62</v>
       </c>
       <c r="B103" s="25" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="C103" s="25" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D103" s="26"/>
       <c r="E103" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -3247,10 +3275,10 @@
         <v>62</v>
       </c>
       <c r="B104" s="25" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C104" s="25" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D104" s="26"/>
       <c r="E104" s="26" t="s">
@@ -3262,10 +3290,10 @@
         <v>62</v>
       </c>
       <c r="B105" s="25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C105" s="25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D105" s="26"/>
       <c r="E105" s="26" t="s">
@@ -3277,10 +3305,10 @@
         <v>62</v>
       </c>
       <c r="B106" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C106" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D106" s="26"/>
       <c r="E106" s="26" t="s">
@@ -3292,29 +3320,34 @@
         <v>62</v>
       </c>
       <c r="B107" s="25" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C107" s="25" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D107" s="26"/>
       <c r="E107" s="26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>62</v>
-      </c>
-      <c r="B108" s="25" t="s">
-        <v>168</v>
-      </c>
-      <c r="C108" s="25" t="s">
-        <v>168</v>
-      </c>
+      <c r="B108" s="25"/>
+      <c r="C108" s="25"/>
       <c r="D108" s="26"/>
-      <c r="E108" s="26" t="s">
-        <v>87</v>
+      <c r="E108" s="26"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F109" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -3322,10 +3355,10 @@
         <v>67</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F110" t="s">
         <v>88</v>
@@ -3336,10 +3369,10 @@
         <v>67</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F111" t="s">
         <v>88</v>
@@ -3350,13 +3383,13 @@
         <v>67</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F112" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -3364,13 +3397,13 @@
         <v>67</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F113" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -3378,13 +3411,13 @@
         <v>67</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F114" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3392,13 +3425,13 @@
         <v>67</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F115" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3406,13 +3439,13 @@
         <v>67</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F116" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3420,10 +3453,10 @@
         <v>67</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F117" t="s">
         <v>93</v>
@@ -3434,10 +3467,10 @@
         <v>67</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F118" t="s">
         <v>93</v>
@@ -3448,10 +3481,10 @@
         <v>67</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F119" t="s">
         <v>93</v>
@@ -3462,13 +3495,13 @@
         <v>67</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F120" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -3476,13 +3509,13 @@
         <v>67</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F121" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3490,13 +3523,13 @@
         <v>67</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>181</v>
+        <v>264</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>181</v>
+        <v>264</v>
       </c>
       <c r="F122" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3504,13 +3537,13 @@
         <v>67</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F123" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3518,13 +3551,13 @@
         <v>67</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F124" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3532,13 +3565,13 @@
         <v>67</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F125" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3546,13 +3579,13 @@
         <v>67</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F126" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -3560,13 +3593,13 @@
         <v>67</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F127" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -3574,13 +3607,13 @@
         <v>67</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F128" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -3588,13 +3621,13 @@
         <v>67</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F129" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
@@ -3602,10 +3635,10 @@
         <v>67</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F130" t="s">
         <v>103</v>
@@ -3616,10 +3649,10 @@
         <v>67</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F131" t="s">
         <v>103</v>
@@ -3630,10 +3663,10 @@
         <v>67</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F132" t="s">
         <v>103</v>
@@ -3644,10 +3677,10 @@
         <v>67</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F133" t="s">
         <v>103</v>
@@ -3658,10 +3691,10 @@
         <v>67</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F134" t="s">
         <v>103</v>
@@ -3672,10 +3705,10 @@
         <v>67</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F135" t="s">
         <v>103</v>
@@ -3686,13 +3719,13 @@
         <v>67</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F136" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -3700,13 +3733,13 @@
         <v>67</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F137" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -3714,13 +3747,13 @@
         <v>67</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F138" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -3728,13 +3761,13 @@
         <v>67</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F139" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -3742,13 +3775,13 @@
         <v>67</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F140" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -3756,13 +3789,13 @@
         <v>67</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F141" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -3770,13 +3803,13 @@
         <v>67</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F142" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -3784,13 +3817,13 @@
         <v>67</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F143" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -3798,13 +3831,13 @@
         <v>67</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F144" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
@@ -3812,13 +3845,13 @@
         <v>67</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F145" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
@@ -3826,13 +3859,13 @@
         <v>67</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F146" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -3840,13 +3873,13 @@
         <v>67</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F147" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -3854,13 +3887,13 @@
         <v>67</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F148" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
@@ -3868,13 +3901,13 @@
         <v>67</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F149" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
@@ -3882,13 +3915,13 @@
         <v>67</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F150" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
@@ -3896,13 +3929,13 @@
         <v>67</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F151" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
@@ -3910,13 +3943,13 @@
         <v>67</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F152" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
@@ -3924,13 +3957,13 @@
         <v>67</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="F153" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
@@ -3938,13 +3971,13 @@
         <v>67</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F154" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
@@ -3952,13 +3985,13 @@
         <v>67</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F155" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
@@ -3966,13 +3999,13 @@
         <v>67</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F156" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
@@ -3980,13 +4013,13 @@
         <v>67</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F157" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
@@ -3994,13 +4027,13 @@
         <v>67</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F158" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
@@ -4008,13 +4041,13 @@
         <v>67</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F159" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
@@ -4022,13 +4055,13 @@
         <v>67</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F160" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
@@ -4036,13 +4069,13 @@
         <v>67</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F161" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -4050,13 +4083,13 @@
         <v>67</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="F162" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -4064,13 +4097,13 @@
         <v>67</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F163" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -4078,13 +4111,13 @@
         <v>67</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F164" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -4092,13 +4125,13 @@
         <v>67</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F165" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -4106,13 +4139,13 @@
         <v>67</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F166" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -4120,13 +4153,13 @@
         <v>67</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="F167" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
@@ -4134,13 +4167,13 @@
         <v>67</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F168" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
@@ -4148,13 +4181,13 @@
         <v>67</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="F169" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -4162,13 +4195,13 @@
         <v>67</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="F170" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -4176,13 +4209,13 @@
         <v>67</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F171" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -4190,13 +4223,13 @@
         <v>67</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="F172" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -4204,13 +4237,13 @@
         <v>67</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F173" t="s">
-        <v>140</v>
+        <v>262</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -4218,10 +4251,10 @@
         <v>67</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F174" t="s">
         <v>141</v>
@@ -4232,10 +4265,10 @@
         <v>67</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="F175" t="s">
         <v>142</v>
@@ -4246,10 +4279,10 @@
         <v>67</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F176" t="s">
         <v>143</v>
@@ -4260,10 +4293,10 @@
         <v>67</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="F177" t="s">
         <v>144</v>
@@ -4274,10 +4307,10 @@
         <v>67</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F178" t="s">
         <v>145</v>
@@ -4288,10 +4321,10 @@
         <v>67</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F179" t="s">
         <v>146</v>
@@ -4302,13 +4335,13 @@
         <v>67</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F180" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -4316,10 +4349,10 @@
         <v>67</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F181" t="s">
         <v>147</v>
@@ -4330,10 +4363,10 @@
         <v>67</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F182" t="s">
         <v>148</v>
@@ -4344,10 +4377,10 @@
         <v>67</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="F183" t="s">
         <v>149</v>
@@ -4358,10 +4391,10 @@
         <v>67</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F184" t="s">
         <v>150</v>
@@ -4372,10 +4405,10 @@
         <v>67</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F185" t="s">
         <v>151</v>
@@ -4386,10 +4419,10 @@
         <v>67</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F186" t="s">
         <v>152</v>
@@ -4400,10 +4433,10 @@
         <v>67</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F187" t="s">
         <v>153</v>
@@ -4414,10 +4447,10 @@
         <v>67</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F188" t="s">
         <v>154</v>
@@ -4428,10 +4461,10 @@
         <v>67</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F189" t="s">
         <v>155</v>
@@ -4442,13 +4475,13 @@
         <v>67</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F190" t="s">
-        <v>156</v>
+        <v>263</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -4456,13 +4489,13 @@
         <v>67</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F191" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -4470,13 +4503,13 @@
         <v>67</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="F192" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -4484,13 +4517,13 @@
         <v>67</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F193" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.25">
@@ -4498,13 +4531,13 @@
         <v>67</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F194" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -4512,13 +4545,13 @@
         <v>67</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F195" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -4526,13 +4559,13 @@
         <v>67</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F196" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -4540,13 +4573,13 @@
         <v>67</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F197" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -4554,13 +4587,13 @@
         <v>67</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F198" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.25">
@@ -4568,13 +4601,13 @@
         <v>67</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F199" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -4582,13 +4615,13 @@
         <v>67</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F200" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -4596,13 +4629,13 @@
         <v>67</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F201" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -4610,33 +4643,24 @@
         <v>67</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F202" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A203" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B203" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="F203" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B8:B11">
-    <sortCondition ref="B8:B11"/>
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B7:B10">
+    <sortCondition ref="B7:B10"/>
   </sortState>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -4647,7 +4671,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4671,10 +4695,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>21</v>

</xml_diff>